<commit_message>
Codigo Arrumado | Faltando conclusão
</commit_message>
<xml_diff>
--- a/spiderman.xlsx
+++ b/spiderman.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thoma\Documents\GitHub\cdados_P2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bruno\Documents\Insper\2º Semestre\Ciência dos Dados\Projeto_2\cdados_P2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44CCF2D0-2517-40F9-96BB-B482D6ECDC1C}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{A9A38B6F-BE40-4229-B6F3-FC05D59D7C9F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="20" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Treinamento" sheetId="1" r:id="rId1"/>
@@ -884,7 +884,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -901,7 +901,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1223,17 +1223,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B301"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A208" workbookViewId="0">
-      <selection activeCell="A156" sqref="A156"/>
+    <sheetView topLeftCell="A83" workbookViewId="0">
+      <selection activeCell="A93" sqref="A93"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="126.1796875" customWidth="1"/>
-    <col min="2" max="2" width="9.6328125" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="126.140625" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1241,7 +1241,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1249,7 +1249,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1257,7 +1257,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1265,7 +1265,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1273,7 +1273,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1281,7 +1281,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1289,7 +1289,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1297,7 +1297,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -1305,7 +1305,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -1313,7 +1313,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -1321,7 +1321,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1329,7 +1329,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -1337,7 +1337,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -1345,7 +1345,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1353,7 +1353,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -1361,7 +1361,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -1369,7 +1369,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -1377,7 +1377,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -1385,7 +1385,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -1393,7 +1393,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -1401,7 +1401,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -1409,7 +1409,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -1417,7 +1417,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -1425,7 +1425,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -1433,7 +1433,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -1441,7 +1441,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -1449,7 +1449,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -1457,7 +1457,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -1465,7 +1465,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -1473,7 +1473,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -1481,7 +1481,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>31</v>
       </c>
@@ -1489,7 +1489,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>32</v>
       </c>
@@ -1497,7 +1497,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>33</v>
       </c>
@@ -1505,7 +1505,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>34</v>
       </c>
@@ -1513,7 +1513,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>35</v>
       </c>
@@ -1521,7 +1521,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>36</v>
       </c>
@@ -1529,7 +1529,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>37</v>
       </c>
@@ -1537,7 +1537,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>38</v>
       </c>
@@ -1545,7 +1545,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>39</v>
       </c>
@@ -1553,7 +1553,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>40</v>
       </c>
@@ -1561,7 +1561,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>41</v>
       </c>
@@ -1569,7 +1569,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>42</v>
       </c>
@@ -1577,7 +1577,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>43</v>
       </c>
@@ -1585,7 +1585,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>44</v>
       </c>
@@ -1593,7 +1593,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>45</v>
       </c>
@@ -1601,7 +1601,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>46</v>
       </c>
@@ -1609,7 +1609,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>47</v>
       </c>
@@ -1617,7 +1617,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>48</v>
       </c>
@@ -1625,7 +1625,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>49</v>
       </c>
@@ -1633,7 +1633,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>50</v>
       </c>
@@ -1641,7 +1641,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>51</v>
       </c>
@@ -1649,7 +1649,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>52</v>
       </c>
@@ -1657,7 +1657,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>53</v>
       </c>
@@ -1665,7 +1665,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>54</v>
       </c>
@@ -1673,7 +1673,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>55</v>
       </c>
@@ -1681,7 +1681,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>56</v>
       </c>
@@ -1689,7 +1689,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>57</v>
       </c>
@@ -1697,7 +1697,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>58</v>
       </c>
@@ -1705,7 +1705,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>59</v>
       </c>
@@ -1713,7 +1713,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>60</v>
       </c>
@@ -1721,7 +1721,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>61</v>
       </c>
@@ -1729,7 +1729,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>62</v>
       </c>
@@ -1737,7 +1737,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>63</v>
       </c>
@@ -1745,7 +1745,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>64</v>
       </c>
@@ -1753,7 +1753,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>65</v>
       </c>
@@ -1761,7 +1761,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>66</v>
       </c>
@@ -1769,7 +1769,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>67</v>
       </c>
@@ -1777,15 +1777,15 @@
         <v>227</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>68</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>69</v>
       </c>
@@ -1793,7 +1793,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>70</v>
       </c>
@@ -1801,15 +1801,15 @@
         <v>227</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>71</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>72</v>
       </c>
@@ -1817,7 +1817,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>73</v>
       </c>
@@ -1825,7 +1825,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>74</v>
       </c>
@@ -1833,7 +1833,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>75</v>
       </c>
@@ -1841,7 +1841,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>76</v>
       </c>
@@ -1849,7 +1849,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>77</v>
       </c>
@@ -1857,7 +1857,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>78</v>
       </c>
@@ -1865,7 +1865,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>79</v>
       </c>
@@ -1873,7 +1873,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>80</v>
       </c>
@@ -1881,7 +1881,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>81</v>
       </c>
@@ -1889,7 +1889,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>82</v>
       </c>
@@ -1897,7 +1897,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>83</v>
       </c>
@@ -1905,7 +1905,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>84</v>
       </c>
@@ -1913,7 +1913,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>85</v>
       </c>
@@ -1921,7 +1921,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>86</v>
       </c>
@@ -1929,7 +1929,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>87</v>
       </c>
@@ -1937,7 +1937,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>88</v>
       </c>
@@ -1945,7 +1945,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>89</v>
       </c>
@@ -1953,7 +1953,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>90</v>
       </c>
@@ -1961,7 +1961,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>91</v>
       </c>
@@ -1969,15 +1969,15 @@
         <v>227</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>92</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>93</v>
       </c>
@@ -1985,7 +1985,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>94</v>
       </c>
@@ -1993,7 +1993,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>95</v>
       </c>
@@ -2001,7 +2001,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>96</v>
       </c>
@@ -2009,7 +2009,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>97</v>
       </c>
@@ -2017,7 +2017,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>98</v>
       </c>
@@ -2025,7 +2025,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>99</v>
       </c>
@@ -2033,7 +2033,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>100</v>
       </c>
@@ -2041,7 +2041,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>101</v>
       </c>
@@ -2049,7 +2049,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>102</v>
       </c>
@@ -2057,7 +2057,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>103</v>
       </c>
@@ -2065,7 +2065,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>104</v>
       </c>
@@ -2073,7 +2073,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>105</v>
       </c>
@@ -2081,7 +2081,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>106</v>
       </c>
@@ -2089,7 +2089,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>107</v>
       </c>
@@ -2097,7 +2097,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>108</v>
       </c>
@@ -2105,7 +2105,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>109</v>
       </c>
@@ -2113,7 +2113,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>110</v>
       </c>
@@ -2121,7 +2121,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>111</v>
       </c>
@@ -2129,15 +2129,15 @@
         <v>227</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>112</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.35">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>113</v>
       </c>
@@ -2145,7 +2145,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>114</v>
       </c>
@@ -2153,7 +2153,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>115</v>
       </c>
@@ -2161,7 +2161,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>116</v>
       </c>
@@ -2169,7 +2169,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>117</v>
       </c>
@@ -2177,7 +2177,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>118</v>
       </c>
@@ -2185,7 +2185,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>119</v>
       </c>
@@ -2193,7 +2193,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>120</v>
       </c>
@@ -2201,7 +2201,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>121</v>
       </c>
@@ -2209,7 +2209,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>122</v>
       </c>
@@ -2217,7 +2217,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>123</v>
       </c>
@@ -2225,7 +2225,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>124</v>
       </c>
@@ -2233,7 +2233,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>125</v>
       </c>
@@ -2241,7 +2241,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>126</v>
       </c>
@@ -2249,7 +2249,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>127</v>
       </c>
@@ -2257,7 +2257,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>127</v>
       </c>
@@ -2265,7 +2265,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>128</v>
       </c>
@@ -2273,7 +2273,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>128</v>
       </c>
@@ -2281,7 +2281,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>129</v>
       </c>
@@ -2289,7 +2289,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>129</v>
       </c>
@@ -2297,7 +2297,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>130</v>
       </c>
@@ -2305,7 +2305,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>130</v>
       </c>
@@ -2313,7 +2313,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>131</v>
       </c>
@@ -2321,7 +2321,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>131</v>
       </c>
@@ -2329,7 +2329,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>132</v>
       </c>
@@ -2337,7 +2337,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>132</v>
       </c>
@@ -2345,7 +2345,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>132</v>
       </c>
@@ -2353,7 +2353,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>133</v>
       </c>
@@ -2361,7 +2361,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>133</v>
       </c>
@@ -2369,7 +2369,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>133</v>
       </c>
@@ -2377,7 +2377,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>134</v>
       </c>
@@ -2385,7 +2385,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>134</v>
       </c>
@@ -2393,7 +2393,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>134</v>
       </c>
@@ -2401,7 +2401,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>134</v>
       </c>
@@ -2409,7 +2409,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>134</v>
       </c>
@@ -2417,7 +2417,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>135</v>
       </c>
@@ -2425,7 +2425,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>135</v>
       </c>
@@ -2433,7 +2433,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>135</v>
       </c>
@@ -2441,7 +2441,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>135</v>
       </c>
@@ -2449,7 +2449,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>135</v>
       </c>
@@ -2457,7 +2457,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>135</v>
       </c>
@@ -2465,7 +2465,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>135</v>
       </c>
@@ -2473,71 +2473,71 @@
         <v>227</v>
       </c>
     </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>136</v>
       </c>
       <c r="B156" s="3" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.35">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>136</v>
       </c>
       <c r="B157" s="3" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.35">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>136</v>
       </c>
       <c r="B158" s="3" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.35">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>136</v>
       </c>
       <c r="B159" s="3" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.35">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>136</v>
       </c>
       <c r="B160" s="3" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.35">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>136</v>
       </c>
       <c r="B161" s="3" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.35">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>136</v>
       </c>
       <c r="B162" s="3" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.35">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>136</v>
       </c>
       <c r="B163" s="3" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.35">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>137</v>
       </c>
@@ -2545,7 +2545,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>137</v>
       </c>
@@ -2553,7 +2553,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>137</v>
       </c>
@@ -2561,7 +2561,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>137</v>
       </c>
@@ -2569,7 +2569,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>137</v>
       </c>
@@ -2577,7 +2577,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>137</v>
       </c>
@@ -2585,7 +2585,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>137</v>
       </c>
@@ -2593,7 +2593,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>137</v>
       </c>
@@ -2601,7 +2601,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>137</v>
       </c>
@@ -2609,7 +2609,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>137</v>
       </c>
@@ -2617,7 +2617,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>137</v>
       </c>
@@ -2625,7 +2625,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>137</v>
       </c>
@@ -2633,7 +2633,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>138</v>
       </c>
@@ -2641,7 +2641,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>138</v>
       </c>
@@ -2649,7 +2649,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>138</v>
       </c>
@@ -2657,7 +2657,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>138</v>
       </c>
@@ -2665,7 +2665,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>138</v>
       </c>
@@ -2673,7 +2673,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>138</v>
       </c>
@@ -2681,7 +2681,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>138</v>
       </c>
@@ -2689,7 +2689,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>138</v>
       </c>
@@ -2697,7 +2697,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>138</v>
       </c>
@@ -2705,7 +2705,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>138</v>
       </c>
@@ -2713,7 +2713,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>138</v>
       </c>
@@ -2721,7 +2721,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>138</v>
       </c>
@@ -2729,7 +2729,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>138</v>
       </c>
@@ -2737,7 +2737,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="189" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>138</v>
       </c>
@@ -2745,7 +2745,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="190" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>139</v>
       </c>
@@ -2753,7 +2753,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="191" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>139</v>
       </c>
@@ -2761,7 +2761,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="192" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>139</v>
       </c>
@@ -2769,7 +2769,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>139</v>
       </c>
@@ -2777,7 +2777,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>139</v>
       </c>
@@ -2785,7 +2785,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>139</v>
       </c>
@@ -2793,7 +2793,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>139</v>
       </c>
@@ -2801,7 +2801,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="197" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>139</v>
       </c>
@@ -2809,7 +2809,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>139</v>
       </c>
@@ -2817,7 +2817,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>139</v>
       </c>
@@ -2825,7 +2825,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>139</v>
       </c>
@@ -2833,7 +2833,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="201" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>139</v>
       </c>
@@ -2841,7 +2841,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="202" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>139</v>
       </c>
@@ -2849,7 +2849,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="203" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>139</v>
       </c>
@@ -2857,7 +2857,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="204" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>139</v>
       </c>
@@ -2865,7 +2865,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="205" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>139</v>
       </c>
@@ -2873,7 +2873,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="206" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>139</v>
       </c>
@@ -2881,7 +2881,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="207" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>139</v>
       </c>
@@ -2889,7 +2889,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="208" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>139</v>
       </c>
@@ -2897,7 +2897,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="209" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>139</v>
       </c>
@@ -2905,7 +2905,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="210" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>139</v>
       </c>
@@ -2913,7 +2913,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="211" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>140</v>
       </c>
@@ -2921,7 +2921,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="212" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>140</v>
       </c>
@@ -2929,7 +2929,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="213" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>140</v>
       </c>
@@ -2937,7 +2937,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="214" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>140</v>
       </c>
@@ -2945,7 +2945,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="215" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>140</v>
       </c>
@@ -2953,7 +2953,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="216" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>140</v>
       </c>
@@ -2961,7 +2961,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="217" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>140</v>
       </c>
@@ -2969,7 +2969,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="218" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>140</v>
       </c>
@@ -2977,7 +2977,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="219" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>140</v>
       </c>
@@ -2985,7 +2985,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="220" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>140</v>
       </c>
@@ -2993,7 +2993,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="221" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>140</v>
       </c>
@@ -3001,7 +3001,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="222" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>140</v>
       </c>
@@ -3009,7 +3009,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="223" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>140</v>
       </c>
@@ -3017,7 +3017,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="224" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>140</v>
       </c>
@@ -3025,7 +3025,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="225" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>140</v>
       </c>
@@ -3033,7 +3033,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="226" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>140</v>
       </c>
@@ -3041,7 +3041,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="227" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>140</v>
       </c>
@@ -3049,7 +3049,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="228" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>140</v>
       </c>
@@ -3057,7 +3057,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="229" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>140</v>
       </c>
@@ -3065,7 +3065,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="230" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>140</v>
       </c>
@@ -3073,7 +3073,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="231" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>140</v>
       </c>
@@ -3081,7 +3081,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="232" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>140</v>
       </c>
@@ -3089,7 +3089,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="233" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>140</v>
       </c>
@@ -3097,7 +3097,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="234" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>140</v>
       </c>
@@ -3105,7 +3105,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="235" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>140</v>
       </c>
@@ -3113,7 +3113,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="236" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>140</v>
       </c>
@@ -3121,7 +3121,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="237" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>140</v>
       </c>
@@ -3129,7 +3129,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="238" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>140</v>
       </c>
@@ -3137,7 +3137,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="239" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>140</v>
       </c>
@@ -3145,7 +3145,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="240" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>140</v>
       </c>
@@ -3153,7 +3153,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="241" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>140</v>
       </c>
@@ -3161,7 +3161,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="242" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>140</v>
       </c>
@@ -3169,7 +3169,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="243" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>140</v>
       </c>
@@ -3177,7 +3177,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="244" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>140</v>
       </c>
@@ -3185,7 +3185,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="245" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="245" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>140</v>
       </c>
@@ -3193,7 +3193,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="246" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="246" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>140</v>
       </c>
@@ -3201,7 +3201,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="247" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="247" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>140</v>
       </c>
@@ -3209,7 +3209,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="248" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="248" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>140</v>
       </c>
@@ -3217,7 +3217,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="249" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="249" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
         <v>140</v>
       </c>
@@ -3225,7 +3225,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="250" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="250" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>140</v>
       </c>
@@ -3233,7 +3233,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="251" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="251" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
         <v>140</v>
       </c>
@@ -3241,7 +3241,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="252" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="252" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
         <v>140</v>
       </c>
@@ -3249,7 +3249,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="253" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="253" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>140</v>
       </c>
@@ -3257,7 +3257,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="254" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="254" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>140</v>
       </c>
@@ -3265,7 +3265,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="255" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="255" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
         <v>140</v>
       </c>
@@ -3273,7 +3273,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="256" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="256" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
         <v>140</v>
       </c>
@@ -3281,7 +3281,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="257" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="257" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
         <v>140</v>
       </c>
@@ -3289,7 +3289,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="258" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="258" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
         <v>140</v>
       </c>
@@ -3297,7 +3297,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="259" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="259" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
         <v>140</v>
       </c>
@@ -3305,7 +3305,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="260" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="260" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
         <v>140</v>
       </c>
@@ -3313,7 +3313,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="261" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="261" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
         <v>140</v>
       </c>
@@ -3321,7 +3321,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="262" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="262" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
         <v>140</v>
       </c>
@@ -3329,7 +3329,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="263" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="263" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
         <v>140</v>
       </c>
@@ -3337,7 +3337,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="264" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="264" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
         <v>140</v>
       </c>
@@ -3345,7 +3345,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="265" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="265" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
         <v>140</v>
       </c>
@@ -3353,7 +3353,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="266" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="266" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
         <v>140</v>
       </c>
@@ -3361,7 +3361,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="267" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="267" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
         <v>140</v>
       </c>
@@ -3369,7 +3369,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="268" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="268" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
         <v>140</v>
       </c>
@@ -3377,7 +3377,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="269" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="269" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
         <v>140</v>
       </c>
@@ -3385,7 +3385,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="270" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="270" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
         <v>140</v>
       </c>
@@ -3393,7 +3393,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="271" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="271" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
         <v>140</v>
       </c>
@@ -3401,7 +3401,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="272" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="272" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
         <v>140</v>
       </c>
@@ -3409,7 +3409,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="273" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="273" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
         <v>140</v>
       </c>
@@ -3417,7 +3417,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="274" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="274" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
         <v>140</v>
       </c>
@@ -3425,7 +3425,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="275" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="275" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
         <v>140</v>
       </c>
@@ -3433,7 +3433,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="276" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="276" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
         <v>140</v>
       </c>
@@ -3441,7 +3441,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="277" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="277" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
         <v>140</v>
       </c>
@@ -3449,7 +3449,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="278" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="278" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
         <v>140</v>
       </c>
@@ -3457,7 +3457,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="279" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="279" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
         <v>140</v>
       </c>
@@ -3465,7 +3465,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="280" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="280" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
         <v>140</v>
       </c>
@@ -3473,7 +3473,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="281" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="281" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
         <v>140</v>
       </c>
@@ -3481,7 +3481,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="282" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="282" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
         <v>140</v>
       </c>
@@ -3489,7 +3489,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="283" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="283" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
         <v>140</v>
       </c>
@@ -3497,7 +3497,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="284" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="284" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
         <v>140</v>
       </c>
@@ -3505,7 +3505,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="285" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="285" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
         <v>140</v>
       </c>
@@ -3513,7 +3513,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="286" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="286" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
         <v>140</v>
       </c>
@@ -3521,7 +3521,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="287" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="287" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
         <v>140</v>
       </c>
@@ -3529,7 +3529,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="288" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="288" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
         <v>140</v>
       </c>
@@ -3537,7 +3537,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="289" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="289" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
         <v>140</v>
       </c>
@@ -3545,7 +3545,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="290" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="290" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
         <v>140</v>
       </c>
@@ -3553,7 +3553,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="291" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="291" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
         <v>140</v>
       </c>
@@ -3561,7 +3561,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="292" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="292" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
         <v>140</v>
       </c>
@@ -3569,7 +3569,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="293" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="293" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
         <v>140</v>
       </c>
@@ -3577,7 +3577,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="294" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="294" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
         <v>140</v>
       </c>
@@ -3585,7 +3585,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="295" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="295" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
         <v>140</v>
       </c>
@@ -3593,7 +3593,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="296" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="296" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
         <v>140</v>
       </c>
@@ -3601,7 +3601,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="297" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="297" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
         <v>140</v>
       </c>
@@ -3609,7 +3609,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="298" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="298" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
         <v>140</v>
       </c>
@@ -3617,7 +3617,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="299" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="299" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
         <v>140</v>
       </c>
@@ -3625,7 +3625,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="300" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="300" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
         <v>140</v>
       </c>
@@ -3633,7 +3633,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="301" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="301" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
         <v>140</v>
       </c>
@@ -3654,17 +3654,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B201"/>
   <sheetViews>
-    <sheetView topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="A55" sqref="A55"/>
+    <sheetView tabSelected="1" topLeftCell="A191" workbookViewId="0">
+      <selection activeCell="B200" sqref="B200"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="119.7265625" customWidth="1"/>
-    <col min="2" max="2" width="9.6328125" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="119.7109375" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>141</v>
       </c>
@@ -3672,7 +3672,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>128</v>
       </c>
@@ -3680,7 +3680,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>142</v>
       </c>
@@ -3688,7 +3688,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>143</v>
       </c>
@@ -3696,7 +3696,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>144</v>
       </c>
@@ -3704,15 +3704,15 @@
         <v>227</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>145</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>146</v>
       </c>
@@ -3720,15 +3720,15 @@
         <v>227</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>147</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>148</v>
       </c>
@@ -3736,7 +3736,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>149</v>
       </c>
@@ -3744,7 +3744,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>150</v>
       </c>
@@ -3752,7 +3752,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>151</v>
       </c>
@@ -3760,7 +3760,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>152</v>
       </c>
@@ -3768,7 +3768,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>153</v>
       </c>
@@ -3776,7 +3776,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>154</v>
       </c>
@@ -3784,7 +3784,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>155</v>
       </c>
@@ -3792,7 +3792,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>156</v>
       </c>
@@ -3800,7 +3800,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>157</v>
       </c>
@@ -3808,7 +3808,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>158</v>
       </c>
@@ -3816,7 +3816,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>159</v>
       </c>
@@ -3824,7 +3824,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>160</v>
       </c>
@@ -3832,7 +3832,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>161</v>
       </c>
@@ -3840,7 +3840,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>162</v>
       </c>
@@ -3848,7 +3848,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>163</v>
       </c>
@@ -3856,7 +3856,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>164</v>
       </c>
@@ -3864,7 +3864,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>165</v>
       </c>
@@ -3872,7 +3872,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>135</v>
       </c>
@@ -3880,7 +3880,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>166</v>
       </c>
@@ -3888,7 +3888,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>167</v>
       </c>
@@ -3896,7 +3896,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>168</v>
       </c>
@@ -3904,7 +3904,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>169</v>
       </c>
@@ -3912,7 +3912,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>170</v>
       </c>
@@ -3920,7 +3920,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>116</v>
       </c>
@@ -3928,7 +3928,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>171</v>
       </c>
@@ -3936,7 +3936,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>172</v>
       </c>
@@ -3944,7 +3944,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>173</v>
       </c>
@@ -3952,7 +3952,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>174</v>
       </c>
@@ -3960,7 +3960,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>175</v>
       </c>
@@ -3968,7 +3968,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>176</v>
       </c>
@@ -3976,7 +3976,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>177</v>
       </c>
@@ -3984,7 +3984,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>178</v>
       </c>
@@ -3992,7 +3992,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>179</v>
       </c>
@@ -4000,7 +4000,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>180</v>
       </c>
@@ -4008,7 +4008,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>181</v>
       </c>
@@ -4016,7 +4016,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>182</v>
       </c>
@@ -4024,7 +4024,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>183</v>
       </c>
@@ -4032,7 +4032,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>184</v>
       </c>
@@ -4040,7 +4040,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>76</v>
       </c>
@@ -4048,7 +4048,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>185</v>
       </c>
@@ -4056,7 +4056,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>186</v>
       </c>
@@ -4064,7 +4064,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>187</v>
       </c>
@@ -4072,7 +4072,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>188</v>
       </c>
@@ -4080,7 +4080,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>189</v>
       </c>
@@ -4088,7 +4088,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>190</v>
       </c>
@@ -4096,7 +4096,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>191</v>
       </c>
@@ -4104,7 +4104,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>71</v>
       </c>
@@ -4112,7 +4112,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>192</v>
       </c>
@@ -4120,7 +4120,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>53</v>
       </c>
@@ -4128,7 +4128,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>193</v>
       </c>
@@ -4136,7 +4136,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>194</v>
       </c>
@@ -4144,7 +4144,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>195</v>
       </c>
@@ -4152,7 +4152,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>196</v>
       </c>
@@ -4160,7 +4160,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>197</v>
       </c>
@@ -4168,7 +4168,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>198</v>
       </c>
@@ -4176,7 +4176,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>199</v>
       </c>
@@ -4184,7 +4184,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>200</v>
       </c>
@@ -4192,7 +4192,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>201</v>
       </c>
@@ -4200,7 +4200,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>202</v>
       </c>
@@ -4208,7 +4208,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>203</v>
       </c>
@@ -4216,7 +4216,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>204</v>
       </c>
@@ -4224,7 +4224,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>205</v>
       </c>
@@ -4232,7 +4232,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>206</v>
       </c>
@@ -4240,7 +4240,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>207</v>
       </c>
@@ -4248,7 +4248,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>208</v>
       </c>
@@ -4256,7 +4256,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>209</v>
       </c>
@@ -4264,7 +4264,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>210</v>
       </c>
@@ -4272,7 +4272,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>211</v>
       </c>
@@ -4280,7 +4280,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>212</v>
       </c>
@@ -4288,7 +4288,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>213</v>
       </c>
@@ -4296,7 +4296,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>214</v>
       </c>
@@ -4304,7 +4304,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>215</v>
       </c>
@@ -4312,7 +4312,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>216</v>
       </c>
@@ -4320,7 +4320,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>37</v>
       </c>
@@ -4328,7 +4328,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>72</v>
       </c>
@@ -4336,15 +4336,15 @@
         <v>227</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>217</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>218</v>
       </c>
@@ -4352,7 +4352,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>219</v>
       </c>
@@ -4360,7 +4360,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>220</v>
       </c>
@@ -4368,7 +4368,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>221</v>
       </c>
@@ -4376,7 +4376,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>222</v>
       </c>
@@ -4384,7 +4384,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>223</v>
       </c>
@@ -4392,7 +4392,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>224</v>
       </c>
@@ -4400,7 +4400,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>133</v>
       </c>
@@ -4408,7 +4408,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>133</v>
       </c>
@@ -4416,7 +4416,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>130</v>
       </c>
@@ -4424,7 +4424,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>130</v>
       </c>
@@ -4432,7 +4432,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>225</v>
       </c>
@@ -4440,7 +4440,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>225</v>
       </c>
@@ -4448,7 +4448,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>132</v>
       </c>
@@ -4456,7 +4456,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>132</v>
       </c>
@@ -4464,7 +4464,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>134</v>
       </c>
@@ -4472,7 +4472,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>134</v>
       </c>
@@ -4480,7 +4480,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>85</v>
       </c>
@@ -4488,7 +4488,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>85</v>
       </c>
@@ -4496,7 +4496,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>85</v>
       </c>
@@ -4504,7 +4504,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>85</v>
       </c>
@@ -4512,7 +4512,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>49</v>
       </c>
@@ -4520,7 +4520,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>49</v>
       </c>
@@ -4528,7 +4528,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>49</v>
       </c>
@@ -4536,7 +4536,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>49</v>
       </c>
@@ -4544,7 +4544,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>137</v>
       </c>
@@ -4552,7 +4552,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>137</v>
       </c>
@@ -4560,7 +4560,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>137</v>
       </c>
@@ -4568,7 +4568,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>137</v>
       </c>
@@ -4576,7 +4576,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>137</v>
       </c>
@@ -4584,7 +4584,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>137</v>
       </c>
@@ -4592,7 +4592,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>137</v>
       </c>
@@ -4600,7 +4600,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>137</v>
       </c>
@@ -4608,7 +4608,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>138</v>
       </c>
@@ -4616,7 +4616,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>138</v>
       </c>
@@ -4624,7 +4624,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>138</v>
       </c>
@@ -4632,7 +4632,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>138</v>
       </c>
@@ -4640,7 +4640,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>138</v>
       </c>
@@ -4648,7 +4648,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>138</v>
       </c>
@@ -4656,7 +4656,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>138</v>
       </c>
@@ -4664,7 +4664,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>138</v>
       </c>
@@ -4672,79 +4672,79 @@
         <v>227</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>136</v>
       </c>
       <c r="B127" s="3" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.35">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>136</v>
       </c>
       <c r="B128" s="3" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.35">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>136</v>
       </c>
       <c r="B129" s="3" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.35">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>136</v>
       </c>
       <c r="B130" s="3" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.35">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>136</v>
       </c>
       <c r="B131" s="3" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.35">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>136</v>
       </c>
       <c r="B132" s="3" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.35">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>136</v>
       </c>
       <c r="B133" s="3" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.35">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>136</v>
       </c>
       <c r="B134" s="3" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.35">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>136</v>
       </c>
       <c r="B135" s="3" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.35">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>139</v>
       </c>
@@ -4752,7 +4752,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>139</v>
       </c>
@@ -4760,7 +4760,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>139</v>
       </c>
@@ -4768,7 +4768,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>139</v>
       </c>
@@ -4776,7 +4776,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>139</v>
       </c>
@@ -4784,7 +4784,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>139</v>
       </c>
@@ -4792,7 +4792,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>139</v>
       </c>
@@ -4800,7 +4800,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>139</v>
       </c>
@@ -4808,7 +4808,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>139</v>
       </c>
@@ -4816,7 +4816,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>139</v>
       </c>
@@ -4824,7 +4824,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>139</v>
       </c>
@@ -4832,7 +4832,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>139</v>
       </c>
@@ -4840,7 +4840,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>139</v>
       </c>
@@ -4848,7 +4848,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>139</v>
       </c>
@@ -4856,7 +4856,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>139</v>
       </c>
@@ -4864,7 +4864,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>139</v>
       </c>
@@ -4872,7 +4872,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>139</v>
       </c>
@@ -4880,7 +4880,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>139</v>
       </c>
@@ -4888,7 +4888,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>139</v>
       </c>
@@ -4896,7 +4896,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>139</v>
       </c>
@@ -4904,7 +4904,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>139</v>
       </c>
@@ -4912,7 +4912,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>139</v>
       </c>
@@ -4920,7 +4920,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>140</v>
       </c>
@@ -4928,7 +4928,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>140</v>
       </c>
@@ -4936,7 +4936,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>140</v>
       </c>
@@ -4944,7 +4944,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>140</v>
       </c>
@@ -4952,7 +4952,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>140</v>
       </c>
@@ -4960,7 +4960,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>140</v>
       </c>
@@ -4968,7 +4968,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>140</v>
       </c>
@@ -4976,7 +4976,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>140</v>
       </c>
@@ -4984,7 +4984,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>140</v>
       </c>
@@ -4992,7 +4992,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>140</v>
       </c>
@@ -5000,7 +5000,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>140</v>
       </c>
@@ -5008,7 +5008,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>140</v>
       </c>
@@ -5016,7 +5016,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>140</v>
       </c>
@@ -5024,7 +5024,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>140</v>
       </c>
@@ -5032,7 +5032,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>140</v>
       </c>
@@ -5040,7 +5040,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>140</v>
       </c>
@@ -5048,7 +5048,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>140</v>
       </c>
@@ -5056,7 +5056,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>140</v>
       </c>
@@ -5064,7 +5064,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>140</v>
       </c>
@@ -5072,7 +5072,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>140</v>
       </c>
@@ -5080,7 +5080,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>140</v>
       </c>
@@ -5088,7 +5088,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>140</v>
       </c>
@@ -5096,7 +5096,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>140</v>
       </c>
@@ -5104,7 +5104,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>140</v>
       </c>
@@ -5112,7 +5112,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>140</v>
       </c>
@@ -5120,7 +5120,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>140</v>
       </c>
@@ -5128,7 +5128,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>140</v>
       </c>
@@ -5136,7 +5136,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>140</v>
       </c>
@@ -5144,7 +5144,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>140</v>
       </c>
@@ -5152,7 +5152,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>140</v>
       </c>
@@ -5160,7 +5160,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>140</v>
       </c>
@@ -5168,7 +5168,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="189" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>140</v>
       </c>
@@ -5176,7 +5176,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="190" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>140</v>
       </c>
@@ -5184,7 +5184,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="191" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>140</v>
       </c>
@@ -5192,7 +5192,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="192" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>140</v>
       </c>
@@ -5200,7 +5200,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>140</v>
       </c>
@@ -5208,7 +5208,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>140</v>
       </c>
@@ -5216,7 +5216,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>140</v>
       </c>
@@ -5224,7 +5224,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>140</v>
       </c>
@@ -5232,7 +5232,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="197" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>140</v>
       </c>
@@ -5240,7 +5240,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>140</v>
       </c>
@@ -5248,7 +5248,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>140</v>
       </c>
@@ -5256,7 +5256,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>140</v>
       </c>
@@ -5264,7 +5264,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="201" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>140</v>
       </c>

</xml_diff>